<commit_message>
Update IP - EX 50 - Tabela dinamica I (Anexo).xlsx
Acompanhamento da aula
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 50 - Tabela dinamica I (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 50 - Tabela dinamica I (Anexo).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC636C2B-BDD1-43E8-9E91-4D0D0AF554F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB5EFDF-C8DE-457B-B480-58B665DB6822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,9 @@
     <sheet name="EXERCÍCIOS" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="6" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="40">
   <si>
     <t>CONCEITO</t>
   </si>
@@ -134,6 +137,24 @@
   </si>
   <si>
     <t>Tabela Dinâmica</t>
+  </si>
+  <si>
+    <t>Total Geral</t>
+  </si>
+  <si>
+    <t>Antônio Total</t>
+  </si>
+  <si>
+    <t>Paulo Total</t>
+  </si>
+  <si>
+    <t>Pedro Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantidade </t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -465,7 +486,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -552,6 +573,15 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Moeda" xfId="2" builtinId="4"/>
@@ -559,7 +589,17 @@
     <cellStyle name="Normal 2" xfId="3" xr:uid="{68AA0FC4-F257-4747-A196-A35E428BCDFE}"/>
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -967,6 +1007,223 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Lorenzo Bianchi" refreshedDate="45727.870865625002" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="6" xr:uid="{62258BE9-EA9F-4744-89F5-69087366F545}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B10:E16" sheet="EXPLICAÇÃO"/>
+  </cacheSource>
+  <cacheFields count="4">
+    <cacheField name="Vendedor" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Pedro"/>
+        <s v="Paulo"/>
+        <s v="Antônio"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Produto" numFmtId="0">
+      <sharedItems count="6">
+        <s v="Impressoras"/>
+        <s v="Scanners"/>
+        <s v="Calculadoras"/>
+        <s v="Desktops"/>
+        <s v="Notebooks"/>
+        <s v="Multifuncionais"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Quantidade" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="6" maxValue="15" count="6">
+        <n v="15"/>
+        <n v="8"/>
+        <n v="10"/>
+        <n v="6"/>
+        <n v="7"/>
+        <n v="11"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Valor" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="10000" maxValue="21000"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="6">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="15000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="20000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <n v="10000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="18000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="4"/>
+    <n v="21000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="5"/>
+    <n v="16000"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{211CEE9D-C704-4160-8C52-5259721CBF18}" name="Tabela dinâmica1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+  <location ref="I10:L20" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
+  <pivotFields count="4">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
+      <items count="7">
+        <item x="2"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0">
+      <items count="7">
+        <item x="3"/>
+        <item x="4"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" numFmtId="164" outline="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="0"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="10">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Quantidade " fld="2" baseField="0" baseItem="0"/>
+    <dataField name="TOTAL" fld="3" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <formats count="3">
+    <format dxfId="2">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
@@ -1256,8 +1513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1447,10 +1704,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:Q18"/>
+  <dimension ref="B1:P20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1462,13 +1719,21 @@
     <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="6" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="str">
         <f>CONTEÚDO!B2</f>
         <v>Tabela Dinâmica</v>
@@ -1486,10 +1751,9 @@
       <c r="M2" s="29"/>
       <c r="N2" s="29"/>
       <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="30"/>
-    </row>
-    <row r="3" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P2" s="30"/>
+    </row>
+    <row r="3" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="31"/>
       <c r="C3" s="32"/>
       <c r="D3" s="32"/>
@@ -1504,10 +1768,9 @@
       <c r="M3" s="32"/>
       <c r="N3" s="32"/>
       <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="33"/>
-    </row>
-    <row r="4" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P3" s="33"/>
+    </row>
+    <row r="4" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="31"/>
       <c r="C4" s="32"/>
       <c r="D4" s="32"/>
@@ -1522,10 +1785,9 @@
       <c r="M4" s="32"/>
       <c r="N4" s="32"/>
       <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="33"/>
-    </row>
-    <row r="5" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P4" s="33"/>
+    </row>
+    <row r="5" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="31"/>
       <c r="C5" s="32"/>
       <c r="D5" s="32"/>
@@ -1540,10 +1802,9 @@
       <c r="M5" s="32"/>
       <c r="N5" s="32"/>
       <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="33"/>
-    </row>
-    <row r="6" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P5" s="33"/>
+    </row>
+    <row r="6" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="34"/>
       <c r="C6" s="35"/>
       <c r="D6" s="35"/>
@@ -1558,10 +1819,9 @@
       <c r="M6" s="35"/>
       <c r="N6" s="35"/>
       <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="36"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P6" s="36"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>0</v>
       </c>
@@ -1569,8 +1829,8 @@
       <c r="D8" s="24"/>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="2:17" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="25" t="s">
         <v>1</v>
       </c>
@@ -1586,8 +1846,20 @@
       <c r="H10" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="I10" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="K10" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
@@ -1600,8 +1872,20 @@
       <c r="E11" s="4">
         <v>15000</v>
       </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="42">
+        <v>10</v>
+      </c>
+      <c r="L11" s="41">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
@@ -1614,8 +1898,17 @@
       <c r="E12" s="4">
         <v>20000</v>
       </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>12</v>
+      </c>
+      <c r="K12" s="42">
+        <v>7</v>
+      </c>
+      <c r="L12" s="41">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
@@ -1628,8 +1921,17 @@
       <c r="E13" s="4">
         <v>10000</v>
       </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" s="42">
+        <v>17</v>
+      </c>
+      <c r="L13" s="41">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>7</v>
       </c>
@@ -1642,8 +1944,20 @@
       <c r="E14" s="4">
         <v>18000</v>
       </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="42">
+        <v>6</v>
+      </c>
+      <c r="L14" s="41">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1656,8 +1970,17 @@
       <c r="E15" s="4">
         <v>21000</v>
       </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>8</v>
+      </c>
+      <c r="K15" s="42">
+        <v>8</v>
+      </c>
+      <c r="L15" s="41">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
@@ -1670,21 +1993,75 @@
       <c r="E16" s="4">
         <v>16000</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" s="42">
+        <v>14</v>
+      </c>
+      <c r="L16" s="41">
+        <v>38000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="42">
+        <v>15</v>
+      </c>
+      <c r="L17" s="41">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="27" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="24"/>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
+      <c r="J18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K18" s="42">
+        <v>11</v>
+      </c>
+      <c r="L18" s="41">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" s="42">
+        <v>26</v>
+      </c>
+      <c r="L19" s="41">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" s="42">
+        <v>57</v>
+      </c>
+      <c r="L20" s="41">
+        <v>100000</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:Q6"/>
+    <mergeCell ref="B2:P6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>